<commit_message>
add more test cases for the transpose optimization and perform more performance comparision
</commit_message>
<xml_diff>
--- a/singleton/use_case/transposeTest/transposeTestResult.xlsx
+++ b/singleton/use_case/transposeTest/transposeTestResult.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="57">
   <si>
     <t>CPU information</t>
   </si>
@@ -84,13 +84,82 @@
     <t>Release</t>
   </si>
   <si>
+    <t>loop tiling, tile size</t>
+  </si>
+  <si>
+    <t>tilesize</t>
+  </si>
+  <si>
     <t>time(ms)</t>
   </si>
   <si>
     <t>speedup</t>
   </si>
   <si>
+    <t>32x32</t>
+  </si>
+  <si>
+    <t>64x64</t>
+  </si>
+  <si>
+    <t>128x128</t>
+  </si>
+  <si>
+    <t>speedup &gt; 1 means there is positive performance gain, otherwise, the performance gain is negative.</t>
+  </si>
+  <si>
+    <t>the higher the speedup, the better performance.</t>
+  </si>
+  <si>
+    <t>Tile size is determined by the size of L1 DCache.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusion: </t>
+  </si>
+  <si>
+    <t>1. for low-dimension matrix, looping tiling is not needed because L1 DCache is big enough.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. for high-dimension matrix, multithreading can improve performance. Tile size 32 has the optimal performance. </t>
+  </si>
+  <si>
+    <t>multithreading, thread num</t>
+  </si>
+  <si>
+    <t>threadNum</t>
+  </si>
+  <si>
+    <t>The thread num is bound by the number of physical core.</t>
+  </si>
+  <si>
+    <t>1. for low-dimension matrix, multithreading is not needed. The more thread num may lead to the negative gain.</t>
+  </si>
+  <si>
+    <t>single optimization method</t>
+  </si>
+  <si>
+    <t>2. for high-dimension matrix, multithreading can improve performance. The more thread num, the better performance.</t>
+  </si>
+  <si>
     <t>naive</t>
+  </si>
+  <si>
+    <t>write consecutively</t>
+  </si>
+  <si>
+    <t>restrict</t>
+  </si>
+  <si>
+    <t>loop tiling,tilesize=32</t>
+  </si>
+  <si>
+    <t>multithreading,threadnum=4</t>
+  </si>
+  <si>
+    <t>Loop tiling is the most effective optimization compared to other optimizations, multithreading comes next, changing the pattern to write consecultively comes third, using restrict to modify the argument comes last.</t>
+  </si>
+  <si>
+    <t>overall</t>
   </si>
   <si>
     <t>opt1(write consecutively)</t>
@@ -99,13 +168,10 @@
     <t>opt2(op1 + restrict)</t>
   </si>
   <si>
-    <t>opt3(op2 + tilesize=64)</t>
+    <t>opt3(op2 + loop tiling,tilesize=32)</t>
   </si>
   <si>
-    <t>opt3(op2 + tilesize=128)</t>
-  </si>
-  <si>
-    <t>opt4(op2 + tilesize=64,threadnum=3)</t>
+    <t>opt4(op3,multithreading,threadnum=4</t>
   </si>
   <si>
     <t>Legend</t>
@@ -120,13 +186,19 @@
     <t>opt1 plus restrict keyword</t>
   </si>
   <si>
-    <t>opt2 plus restrict keyword and loop titling (tile size 64)</t>
+    <t>opt3(op2 + tilesize=32)</t>
   </si>
   <si>
-    <t>opt2 plus restrict keyword and loop titling (tile size 128)</t>
+    <t>opt2 plus loop titling (tile size 32)</t>
   </si>
   <si>
-    <t>opt2 plus restrict keyword and loop titling (tile size 64) and multithreading (thread num 3)</t>
+    <t>opt4(op3,threadnum=4)</t>
+  </si>
+  <si>
+    <t>opt3 plus multithreading (thread num 4)</t>
+  </si>
+  <si>
+    <t>With the help of all optimizations, the speedup can achieve almost 7.</t>
   </si>
 </sst>
 </file>
@@ -749,18 +821,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -858,7 +933,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>matrix transpose speedup using different optimizations</a:t>
+              <a:t>matrix transpose speedup using different optimizations (overall)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" altLang="zh-CN"/>
           </a:p>
@@ -893,7 +968,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>result!$A$1</c:f>
+              <c:f>result!$A$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -917,7 +992,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>result!$B$13:$B$18</c:f>
+              <c:f>result!$B$96:$B$101</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -930,20 +1005,17 @@
                   <c:v>opt2(op1 + restrict)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>opt3(op2 + tilesize=64)</c:v>
+                  <c:v>opt3(op2 + loop tiling,tilesize=32)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>opt3(op2 + tilesize=128)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>opt4(op2 + tilesize=64,threadnum=3)</c:v>
+                  <c:v>opt4(op3,multithreading,threadnum=4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>result!$D$3:$D$8</c:f>
+              <c:f>result!$D$86:$D$91</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="6"/>
@@ -951,19 +1023,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.03669724770642</c:v>
+                  <c:v>1.10869565217391</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.39506172839506</c:v>
+                  <c:v>1.24390243902439</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.59154929577465</c:v>
+                  <c:v>1.41666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.46753246753247</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.71212121212121</c:v>
+                  <c:v>2.26666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,7 +1043,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>result!$A$11</c:f>
+              <c:f>result!$A$94</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -998,7 +1067,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>result!$B$13:$B$18</c:f>
+              <c:f>result!$B$96:$B$101</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1011,20 +1080,17 @@
                   <c:v>opt2(op1 + restrict)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>opt3(op2 + tilesize=64)</c:v>
+                  <c:v>opt3(op2 + loop tiling,tilesize=32)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>opt3(op2 + tilesize=128)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>opt4(op2 + tilesize=64,threadnum=3)</c:v>
+                  <c:v>opt4(op3,multithreading,threadnum=4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>result!$D$13:$D$18</c:f>
+              <c:f>result!$D$96:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="6"/>
@@ -1032,19 +1098,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.31802785095973</c:v>
+                  <c:v>1.3126213592233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6086357372531</c:v>
+                  <c:v>1.45189003436426</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.64791666666667</c:v>
+                  <c:v>3.62272240085745</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0719298245614</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.66666666666667</c:v>
+                  <c:v>4.89146164978292</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1055,7 +1118,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>result!$A$21</c:f>
+              <c:f>result!$A$104</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1079,7 +1142,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>result!$B$13:$B$18</c:f>
+              <c:f>result!$B$96:$B$101</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1092,20 +1155,17 @@
                   <c:v>opt2(op1 + restrict)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>opt3(op2 + tilesize=64)</c:v>
+                  <c:v>opt3(op2 + loop tiling,tilesize=32)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>opt3(op2 + tilesize=128)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>opt4(op2 + tilesize=64,threadnum=3)</c:v>
+                  <c:v>opt4(op3,multithreading,threadnum=4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>result!$D$23:$D$28</c:f>
+              <c:f>result!$D$106:$D$111</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
                 <c:ptCount val="6"/>
@@ -1113,19 +1173,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.31451009723261</c:v>
+                  <c:v>1.54690350456073</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.59772727272727</c:v>
+                  <c:v>1.68120630282792</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.92550977944236</c:v>
+                  <c:v>3.01930284857571</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9249726177437</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.27366787377134</c:v>
+                  <c:v>6.91162591162591</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1324,6 +1381,1426 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>matrix transpose speedup using loop tiling with different tile size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.197593167701863"/>
+          <c:y val="0.0349854227405248"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0339202139514152"/>
+          <c:y val="0.171043417366947"/>
+          <c:w val="0.940301612064483"/>
+          <c:h val="0.701750700280112"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$84</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256x256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>result!$B$5:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32x32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64x64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128x128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256x256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$5:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02247191011236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.722222222222222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$94</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>result!$B$5:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32x32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64x64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128x128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256x256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$15:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.468597348220516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.536770583533174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.474055771267208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048x2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>result!$B$5:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32x32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64x64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128x128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256x256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$25:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.04074922785693</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.855318103660034</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.716117090560088</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="246"/>
+        <c:overlap val="-28"/>
+        <c:axId val="740971811"/>
+        <c:axId val="573367126"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="740971811"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573367126"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573367126"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90200"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740971811"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>matrix transpose speedup using multithreading with different thread num</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.197593167701863"/>
+          <c:y val="0.0349854227405248"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$84</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256x256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>result!$B$36:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$36:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.816753926701571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.715596330275229</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.597701149425287</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$94</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>result!$B$36:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$44:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.37430786267996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.73647388059701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.71015158474966</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048x2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>result!$B$36:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$52:$D$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.69814191024666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.12712671838846</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.36931473620376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="246"/>
+        <c:overlap val="-28"/>
+        <c:axId val="740971811"/>
+        <c:axId val="573367126"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="740971811"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573367126"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573367126"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90200"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740971811"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="zh-CN" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>matrix transpose speedup using different optimizations (single optimization)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.197593167701863"/>
+          <c:y val="0.0349854227405248"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$84</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256x256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>result!$B$61:$B$65</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>naive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>write consecutively</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>restrict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>loop tiling,tilesize=32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>multithreading,threadnum=4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$61:$D$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.30232558139535</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.09803921568627</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42911877394636</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$94</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>result!$B$61:$B$65</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>naive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>write consecutively</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>restrict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>loop tiling,tilesize=32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>multithreading,threadnum=4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$69:$D$73</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21988174427199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.831276756484513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.45793000744602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.51630684428112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>result!$A$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048x2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>result!$B$61:$B$65</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>naive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>write consecutively</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>restrict</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>loop tiling,tilesize=32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>multithreading,threadnum=4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>result!$D$77:$D$81</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.55105666729007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.05475009538344</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.58788052843194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.51470588235294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="246"/>
+        <c:overlap val="-28"/>
+        <c:axId val="740971811"/>
+        <c:axId val="573367126"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="740971811"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573367126"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573367126"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90200"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740971811"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1364,7 +2841,1657 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10001">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="90200"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10001">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="90200"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10001">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="90200"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10001">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1927,13 +5054,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1521460</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>172720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -1942,12 +5069,102 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6390640" y="1087120"/>
+        <a:off x="7898130" y="16266160"/>
         <a:ext cx="8536940" cy="3702685"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490220</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>45085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7992110" y="548640"/>
+        <a:ext cx="8536940" cy="3702685"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490220</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>45085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7992110" y="5852160"/>
+        <a:ext cx="8536940" cy="3702685"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490220</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>45085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="图表 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7992110" y="10789920"/>
+        <a:ext cx="8536940" cy="3702685"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2209,7 +5426,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -2316,324 +5533,949 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="40.1111111111111" customWidth="1"/>
-    <col min="4" max="4" width="12.8888888888889" style="1"/>
+    <col min="1" max="1" width="30.9814814814815" customWidth="1"/>
+    <col min="2" max="2" width="40.1111111111111" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.8888888888889" style="2"/>
     <col min="5" max="5" width="23.5555555555556" customWidth="1"/>
     <col min="6" max="6" width="32.1111111111111" customWidth="1"/>
     <col min="7" max="7" width="49.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="3:4">
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    <row r="4" spans="2:4">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
-        <v>0.113</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>0.091</v>
+      </c>
+      <c r="D5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
+    <row r="6" spans="2:4">
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>0.089</v>
+      </c>
+      <c r="D6" s="2">
+        <f>$C$5/C6</f>
+        <v>1.02247191011236</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>0.091</v>
+      </c>
+      <c r="D7" s="2">
+        <f>$C$5/C7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.126</v>
+      </c>
+      <c r="D8" s="2">
+        <f>$C$5/C8</f>
+        <v>0.722222222222222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
-        <v>0.109</v>
-      </c>
-      <c r="D4" s="1">
-        <f>$C$3/C4</f>
-        <v>1.03669724770642</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" t="s">
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5">
-        <v>0.081</v>
-      </c>
-      <c r="D5" s="1">
-        <f>$C$3/C5</f>
-        <v>1.39506172839506</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" t="s">
+      <c r="C15">
+        <v>1.343</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
-        <v>0.071</v>
-      </c>
-      <c r="D6" s="1">
-        <f>$C$3/C6</f>
-        <v>1.59154929577465</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="s">
+      <c r="C16">
+        <v>2.866</v>
+      </c>
+      <c r="D16" s="2">
+        <f>$C$15/C16</f>
+        <v>0.468597348220516</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>0.077</v>
-      </c>
-      <c r="D7" s="1">
-        <f>$C$3/C7</f>
-        <v>1.46753246753247</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" t="s">
+      <c r="C17">
+        <v>2.502</v>
+      </c>
+      <c r="D17" s="2">
+        <f>$C$15/C17</f>
+        <v>0.536770583533174</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>2.833</v>
+      </c>
+      <c r="D18" s="2">
+        <f>$C$15/C18</f>
+        <v>0.474055771267208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>10.446</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
-        <v>0.066</v>
-      </c>
-      <c r="D8" s="1">
-        <f>$C$3/C8</f>
-        <v>1.71212121212121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4">
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>3.502</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>2.657</v>
-      </c>
-      <c r="D14" s="1">
-        <f>$C$13/C14</f>
-        <v>1.31802785095973</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>2.177</v>
-      </c>
-      <c r="D15" s="1">
-        <f>$C$13/C15</f>
-        <v>1.6086357372531</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" t="s">
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16">
-        <v>0.96</v>
-      </c>
-      <c r="D16" s="1">
-        <f>$C$13/C16</f>
-        <v>3.64791666666667</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" t="s">
+      <c r="C26">
+        <v>10.037</v>
+      </c>
+      <c r="D26" s="2">
+        <f>$C$25/C26</f>
+        <v>1.04074922785693</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
-        <v>1.14</v>
-      </c>
-      <c r="D17" s="1">
-        <f>$C$13/C17</f>
-        <v>3.0719298245614</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18">
-        <v>0.618</v>
-      </c>
-      <c r="D18" s="1">
-        <f>$C$13/C18</f>
-        <v>5.66666666666667</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4">
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23">
-        <v>14.06</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24">
-        <v>10.696</v>
-      </c>
-      <c r="D24" s="1">
-        <f>$C$23/C24</f>
-        <v>1.31451009723261</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25">
-        <v>8.8</v>
-      </c>
-      <c r="D25" s="1">
-        <f>$C$23/C25</f>
-        <v>1.59772727272727</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26">
-        <v>4.806</v>
-      </c>
-      <c r="D26" s="1">
-        <f>$C$23/C26</f>
-        <v>2.92550977944236</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
       <c r="C27">
-        <v>7.304</v>
-      </c>
-      <c r="D27" s="1">
-        <f>$C$23/C27</f>
-        <v>1.9249726177437</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" t="s">
-        <v>25</v>
+        <v>12.213</v>
+      </c>
+      <c r="D27" s="2">
+        <f>$C$25/C27</f>
+        <v>0.855318103660034</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>1.933</v>
-      </c>
-      <c r="D28" s="1">
-        <f>$C$23/C28</f>
-        <v>7.27366787377134</v>
+        <v>14.587</v>
+      </c>
+      <c r="D28" s="2">
+        <f>$C$25/C28</f>
+        <v>0.716117090560088</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="6:6">
       <c r="F29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" ht="28.8" spans="6:7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6">
       <c r="F30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="6:7">
-      <c r="F31" t="s">
+      <c r="D35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G31" t="s">
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0.156</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>0.191</v>
+      </c>
+      <c r="D37" s="2">
+        <f>$C$36/C37</f>
+        <v>0.816753926701571</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="1">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>0.218</v>
+      </c>
+      <c r="D38" s="2">
+        <f>$C$36/C38</f>
+        <v>0.715596330275229</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="1">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>0.261</v>
+      </c>
+      <c r="D39" s="2">
+        <f>$C$36/C39</f>
+        <v>0.597701149425287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>3.723</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2.709</v>
+      </c>
+      <c r="D45" s="2">
+        <f>$C$44/C45</f>
+        <v>1.37430786267996</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>2.144</v>
+      </c>
+      <c r="D46" s="2">
+        <f>$C$44/C46</f>
+        <v>1.73647388059701</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="1">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>2.177</v>
+      </c>
+      <c r="D47" s="2">
+        <f>$C$44/C47</f>
+        <v>1.71015158474966</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>15.628</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>9.203</v>
+      </c>
+      <c r="D53" s="2">
+        <f>$C$52/C53</f>
+        <v>1.69814191024666</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>7.347</v>
+      </c>
+      <c r="D54" s="2">
+        <f>$C$52/C54</f>
+        <v>2.12712671838846</v>
+      </c>
+      <c r="F54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="1">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>6.596</v>
+      </c>
+      <c r="D55" s="2">
+        <f>$C$52/C55</f>
+        <v>2.36931473620376</v>
+      </c>
+      <c r="F55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="6:7">
-      <c r="F32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7">
-      <c r="F33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7">
-      <c r="F34" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="6:7">
-      <c r="F35" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" t="s">
-        <v>32</v>
+    <row r="56" spans="6:6">
+      <c r="F56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4">
+      <c r="C60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61">
+        <v>0.112</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62">
+        <v>0.086</v>
+      </c>
+      <c r="D62" s="2">
+        <f>$C$61/C62</f>
+        <v>1.30232558139535</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63">
+        <v>0.102</v>
+      </c>
+      <c r="D63" s="2">
+        <f>$C$61/C63</f>
+        <v>1.09803921568627</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64">
+        <v>0.091</v>
+      </c>
+      <c r="D64" s="2">
+        <f>$C$61/C64</f>
+        <v>1.23076923076923</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65">
+        <v>0.261</v>
+      </c>
+      <c r="D65" s="2">
+        <f>$C$61/C65</f>
+        <v>0.42911877394636</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4">
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69">
+        <v>3.301</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70">
+        <v>2.706</v>
+      </c>
+      <c r="D70" s="2">
+        <f>$C$69/C70</f>
+        <v>1.21988174427199</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71">
+        <v>3.971</v>
+      </c>
+      <c r="D71" s="2">
+        <f>$C$69/C71</f>
+        <v>0.831276756484513</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72">
+        <v>1.343</v>
+      </c>
+      <c r="D72" s="2">
+        <f>$C$69/C72</f>
+        <v>2.45793000744602</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C73">
+        <v>2.177</v>
+      </c>
+      <c r="D73" s="2">
+        <f>$C$69/C73</f>
+        <v>1.51630684428112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4">
+      <c r="C76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77">
+        <v>16.587</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78">
+        <v>10.694</v>
+      </c>
+      <c r="D78" s="2">
+        <f>$C$77/C78</f>
+        <v>1.55105666729007</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79">
+        <v>15.726</v>
+      </c>
+      <c r="D79" s="2">
+        <f>$C$77/C79</f>
+        <v>1.05475009538344</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80">
+        <v>10.446</v>
+      </c>
+      <c r="D80" s="2">
+        <f>$C$77/C80</f>
+        <v>1.58788052843194</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81">
+        <v>6.596</v>
+      </c>
+      <c r="D81" s="2">
+        <f>$C$77/C81</f>
+        <v>2.51470588235294</v>
+      </c>
+      <c r="F81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6">
+      <c r="F82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4">
+      <c r="C85" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C86">
+        <v>0.102</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87">
+        <v>0.092</v>
+      </c>
+      <c r="D87" s="2">
+        <f>$C$86/C87</f>
+        <v>1.10869565217391</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88">
+        <v>0.082</v>
+      </c>
+      <c r="D88" s="2">
+        <f>$C$86/C88</f>
+        <v>1.24390243902439</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89">
+        <v>0.072</v>
+      </c>
+      <c r="D89" s="2">
+        <f>$C$86/C89</f>
+        <v>1.41666666666667</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C90">
+        <v>0.045</v>
+      </c>
+      <c r="D90" s="2">
+        <f>$C$86/C90</f>
+        <v>2.26666666666667</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4">
+      <c r="C95" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C96">
+        <v>3.38</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97">
+        <v>2.575</v>
+      </c>
+      <c r="D97" s="2">
+        <f>$C$96/C97</f>
+        <v>1.3126213592233</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98">
+        <v>2.328</v>
+      </c>
+      <c r="D98" s="2">
+        <f>$C$96/C98</f>
+        <v>1.45189003436426</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99">
+        <v>0.933</v>
+      </c>
+      <c r="D99" s="2">
+        <f>$C$96/C99</f>
+        <v>3.62272240085745</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="B100" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100">
+        <v>0.691</v>
+      </c>
+      <c r="D100" s="2">
+        <f>$C$96/C100</f>
+        <v>4.89146164978292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4">
+      <c r="C105" t="s">
+        <v>20</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106">
+        <v>16.111</v>
+      </c>
+      <c r="D106" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="B107" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107">
+        <v>10.415</v>
+      </c>
+      <c r="D107" s="2">
+        <f>$C$106/C107</f>
+        <v>1.54690350456073</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C108">
+        <v>9.583</v>
+      </c>
+      <c r="D108" s="2">
+        <f>$C$106/C108</f>
+        <v>1.68120630282792</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C109">
+        <v>5.336</v>
+      </c>
+      <c r="D109" s="2">
+        <f>$C$106/C109</f>
+        <v>3.01930284857571</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C110">
+        <v>2.331</v>
+      </c>
+      <c r="D110" s="2">
+        <f>$C$106/C110</f>
+        <v>6.91162591162591</v>
+      </c>
+    </row>
+    <row r="112" spans="6:6">
+      <c r="F112" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="113" ht="28.8" spans="6:7">
+      <c r="F113" t="s">
+        <v>37</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" spans="6:7">
+      <c r="F114" t="s">
+        <v>44</v>
+      </c>
+      <c r="G114" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="6:7">
+      <c r="F115" t="s">
+        <v>45</v>
+      </c>
+      <c r="G115" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="116" spans="6:7">
+      <c r="F116" t="s">
+        <v>52</v>
+      </c>
+      <c r="G116" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="117" spans="6:7">
+      <c r="F117" t="s">
+        <v>54</v>
+      </c>
+      <c r="G117" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="119" spans="6:6">
+      <c r="F119" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" spans="6:6">
+      <c r="F120" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>